<commit_message>
looks good, no error
</commit_message>
<xml_diff>
--- a/Stata/Outputs/hh_mem_codebook.xlsx
+++ b/Stata/Outputs/hh_mem_codebook.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2873" uniqueCount="2600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="3094" uniqueCount="2600">
   <si>
     <t>name</t>
   </si>
@@ -7820,7 +7820,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -7857,8 +7857,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -7866,7 +7869,7 @@
         <v>2422</v>
       </c>
       <c r="B1" t="s">
-        <v>2438</v>
+        <v>2583</v>
       </c>
       <c r="C1" t="s">
         <v>2454</v>
@@ -7898,39 +7901,39 @@
         <v>2439</v>
       </c>
       <c r="C2" t="s">
-        <v>2455</v>
+        <v>2528</v>
       </c>
       <c r="D2" t="s">
-        <v>2471</v>
+        <v>2565</v>
       </c>
       <c r="E2" t="s">
-        <v>2487</v>
+        <v>2561</v>
       </c>
       <c r="F2" t="s">
-        <v>2503</v>
+        <v>2561</v>
       </c>
       <c r="G2" t="s">
-        <v>2519</v>
+        <v>2561</v>
       </c>
       <c r="H2" t="s">
-        <v>2531</v>
+        <v>2561</v>
       </c>
       <c r="I2" t="s">
-        <v>2547</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2424</v>
+        <v>2561</v>
       </c>
       <c r="B3" t="s">
-        <v>2440</v>
+        <v>2561</v>
       </c>
       <c r="C3" t="s">
-        <v>2456</v>
+        <v>2561</v>
       </c>
       <c r="D3" t="s">
-        <v>2472</v>
+        <v>2561</v>
       </c>
       <c r="E3" t="s">
         <v>2488</v>
@@ -7939,27 +7942,27 @@
         <v>2504</v>
       </c>
       <c r="G3" t="s">
-        <v>2520</v>
+        <v>2528</v>
       </c>
       <c r="H3" t="s">
-        <v>2532</v>
+        <v>2561</v>
       </c>
       <c r="I3" t="s">
-        <v>2548</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2425</v>
+        <v>2561</v>
       </c>
       <c r="B4" t="s">
-        <v>2441</v>
+        <v>2561</v>
       </c>
       <c r="C4" t="s">
-        <v>2457</v>
+        <v>2561</v>
       </c>
       <c r="D4" t="s">
-        <v>2473</v>
+        <v>2561</v>
       </c>
       <c r="E4" t="s">
         <v>2489</v>
@@ -7968,27 +7971,27 @@
         <v>2505</v>
       </c>
       <c r="G4" t="s">
-        <v>2521</v>
+        <v>2529</v>
       </c>
       <c r="H4" t="s">
-        <v>2533</v>
+        <v>2561</v>
       </c>
       <c r="I4" t="s">
-        <v>2549</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2426</v>
+        <v>2561</v>
       </c>
       <c r="B5" t="s">
-        <v>2442</v>
+        <v>2561</v>
       </c>
       <c r="C5" t="s">
-        <v>2458</v>
+        <v>2561</v>
       </c>
       <c r="D5" t="s">
-        <v>2474</v>
+        <v>2561</v>
       </c>
       <c r="E5" t="s">
         <v>2490</v>
@@ -7997,27 +8000,27 @@
         <v>2506</v>
       </c>
       <c r="G5" t="s">
-        <v>2521</v>
+        <v>2529</v>
       </c>
       <c r="H5" t="s">
-        <v>2534</v>
+        <v>2561</v>
       </c>
       <c r="I5" t="s">
-        <v>2550</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2427</v>
+        <v>2561</v>
       </c>
       <c r="B6" t="s">
-        <v>2443</v>
+        <v>2561</v>
       </c>
       <c r="C6" t="s">
-        <v>2459</v>
+        <v>2561</v>
       </c>
       <c r="D6" t="s">
-        <v>2475</v>
+        <v>2561</v>
       </c>
       <c r="E6" t="s">
         <v>2491</v>
@@ -8026,300 +8029,300 @@
         <v>2507</v>
       </c>
       <c r="G6" t="s">
-        <v>2522</v>
+        <v>2528</v>
       </c>
       <c r="H6" t="s">
-        <v>2535</v>
+        <v>2561</v>
       </c>
       <c r="I6" t="s">
-        <v>2551</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2428</v>
+        <v>2561</v>
       </c>
       <c r="B7" t="s">
-        <v>2444</v>
+        <v>2561</v>
       </c>
       <c r="C7" t="s">
-        <v>2460</v>
+        <v>2561</v>
       </c>
       <c r="D7" t="s">
-        <v>2476</v>
+        <v>2561</v>
       </c>
       <c r="E7" t="s">
         <v>2492</v>
       </c>
       <c r="F7" t="s">
-        <v>2508</v>
+        <v>2561</v>
       </c>
       <c r="G7" t="s">
-        <v>2522</v>
+        <v>2528</v>
       </c>
       <c r="H7" t="s">
-        <v>2536</v>
+        <v>2563</v>
       </c>
       <c r="I7" t="s">
-        <v>2552</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>2429</v>
+        <v>2561</v>
       </c>
       <c r="B8" t="s">
-        <v>2445</v>
+        <v>2561</v>
       </c>
       <c r="C8" t="s">
-        <v>2461</v>
+        <v>2561</v>
       </c>
       <c r="D8" t="s">
-        <v>2477</v>
+        <v>2561</v>
       </c>
       <c r="E8" t="s">
         <v>2493</v>
       </c>
       <c r="F8" t="s">
-        <v>2509</v>
+        <v>2561</v>
       </c>
       <c r="G8" t="s">
-        <v>2523</v>
+        <v>2529</v>
       </c>
       <c r="H8" t="s">
-        <v>2537</v>
+        <v>2561</v>
       </c>
       <c r="I8" t="s">
-        <v>2553</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>2430</v>
+        <v>2561</v>
       </c>
       <c r="B9" t="s">
-        <v>2446</v>
+        <v>2561</v>
       </c>
       <c r="C9" t="s">
-        <v>2462</v>
+        <v>2561</v>
       </c>
       <c r="D9" t="s">
-        <v>2478</v>
+        <v>2561</v>
       </c>
       <c r="E9" t="s">
         <v>2494</v>
       </c>
       <c r="F9" t="s">
-        <v>2510</v>
+        <v>2561</v>
       </c>
       <c r="G9" t="s">
-        <v>2524</v>
+        <v>2528</v>
       </c>
       <c r="H9" t="s">
-        <v>2538</v>
+        <v>2565</v>
       </c>
       <c r="I9" t="s">
-        <v>2554</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>2431</v>
+        <v>2561</v>
       </c>
       <c r="B10" t="s">
-        <v>2447</v>
+        <v>2561</v>
       </c>
       <c r="C10" t="s">
-        <v>2463</v>
+        <v>2561</v>
       </c>
       <c r="D10" t="s">
-        <v>2479</v>
+        <v>2561</v>
       </c>
       <c r="E10" t="s">
         <v>2495</v>
       </c>
       <c r="F10" t="s">
-        <v>2511</v>
+        <v>2561</v>
       </c>
       <c r="G10" t="s">
-        <v>2525</v>
+        <v>2529</v>
       </c>
       <c r="H10" t="s">
-        <v>2539</v>
+        <v>2561</v>
       </c>
       <c r="I10" t="s">
-        <v>2555</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>2432</v>
+        <v>2561</v>
       </c>
       <c r="B11" t="s">
-        <v>2448</v>
+        <v>2561</v>
       </c>
       <c r="C11" t="s">
-        <v>2464</v>
+        <v>2561</v>
       </c>
       <c r="D11" t="s">
-        <v>2480</v>
+        <v>2561</v>
       </c>
       <c r="E11" t="s">
         <v>2496</v>
       </c>
       <c r="F11" t="s">
-        <v>2512</v>
+        <v>2561</v>
       </c>
       <c r="G11" t="s">
-        <v>2526</v>
+        <v>2528</v>
       </c>
       <c r="H11" t="s">
-        <v>2540</v>
+        <v>2565</v>
       </c>
       <c r="I11" t="s">
-        <v>2556</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>2433</v>
+        <v>2561</v>
       </c>
       <c r="B12" t="s">
-        <v>2449</v>
+        <v>2561</v>
       </c>
       <c r="C12" t="s">
-        <v>2465</v>
+        <v>2561</v>
       </c>
       <c r="D12" t="s">
-        <v>2481</v>
+        <v>2561</v>
       </c>
       <c r="E12" t="s">
         <v>2497</v>
       </c>
       <c r="F12" t="s">
-        <v>2513</v>
+        <v>2561</v>
       </c>
       <c r="G12" t="s">
-        <v>2526</v>
+        <v>2528</v>
       </c>
       <c r="H12" t="s">
-        <v>2541</v>
+        <v>2561</v>
       </c>
       <c r="I12" t="s">
-        <v>2557</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>2434</v>
+        <v>2561</v>
       </c>
       <c r="B13" t="s">
-        <v>2450</v>
+        <v>2561</v>
       </c>
       <c r="C13" t="s">
-        <v>2466</v>
+        <v>2561</v>
       </c>
       <c r="D13" t="s">
-        <v>2482</v>
+        <v>2561</v>
       </c>
       <c r="E13" t="s">
         <v>2498</v>
       </c>
       <c r="F13" t="s">
-        <v>2514</v>
+        <v>2561</v>
       </c>
       <c r="G13" t="s">
-        <v>2526</v>
+        <v>2528</v>
       </c>
       <c r="H13" t="s">
-        <v>2542</v>
+        <v>2564</v>
       </c>
       <c r="I13" t="s">
-        <v>2558</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>2435</v>
+        <v>2561</v>
       </c>
       <c r="B14" t="s">
-        <v>2451</v>
+        <v>2561</v>
       </c>
       <c r="C14" t="s">
-        <v>2467</v>
+        <v>2561</v>
       </c>
       <c r="D14" t="s">
-        <v>2483</v>
+        <v>2561</v>
       </c>
       <c r="E14" t="s">
         <v>2499</v>
       </c>
       <c r="F14" t="s">
-        <v>2515</v>
+        <v>2561</v>
       </c>
       <c r="G14" t="s">
         <v>2527</v>
       </c>
       <c r="H14" t="s">
-        <v>2543</v>
+        <v>2561</v>
       </c>
       <c r="I14" t="s">
-        <v>2559</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>2436</v>
+        <v>2561</v>
       </c>
       <c r="B15" t="s">
-        <v>2452</v>
+        <v>2561</v>
       </c>
       <c r="C15" t="s">
-        <v>2468</v>
+        <v>2561</v>
       </c>
       <c r="D15" t="s">
-        <v>2484</v>
+        <v>2561</v>
       </c>
       <c r="E15" t="s">
         <v>2500</v>
       </c>
       <c r="F15" t="s">
-        <v>2516</v>
+        <v>2561</v>
       </c>
       <c r="G15" t="s">
         <v>2528</v>
       </c>
       <c r="H15" t="s">
-        <v>2544</v>
+        <v>2565</v>
       </c>
       <c r="I15" t="s">
-        <v>2560</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>2437</v>
+        <v>2561</v>
       </c>
       <c r="B16" t="s">
-        <v>2453</v>
+        <v>2561</v>
       </c>
       <c r="C16" t="s">
-        <v>2469</v>
+        <v>2561</v>
       </c>
       <c r="D16" t="s">
-        <v>2485</v>
+        <v>2561</v>
       </c>
       <c r="E16" t="s">
         <v>2501</v>
       </c>
       <c r="F16" t="s">
-        <v>2517</v>
+        <v>2561</v>
       </c>
       <c r="G16" t="s">
         <v>2529</v>
       </c>
       <c r="H16" t="s">
-        <v>2545</v>
+        <v>2561</v>
       </c>
       <c r="I16" t="s">
         <v>2561</v>
@@ -8330,74 +8333,77 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>2408</v>
+        <v>2562</v>
       </c>
       <c r="B1" t="s">
-        <v>2410</v>
+        <v>2566</v>
       </c>
       <c r="C1" t="s">
-        <v>2416</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2409</v>
+        <v>2565</v>
       </c>
       <c r="B2" t="s">
-        <v>2411</v>
+        <v>2578</v>
       </c>
       <c r="C2" t="s">
-        <v>2417</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2409</v>
+        <v>2565</v>
       </c>
       <c r="B3" t="s">
-        <v>2412</v>
+        <v>2579</v>
       </c>
       <c r="C3" t="s">
-        <v>2418</v>
+        <v>2596</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2409</v>
+        <v>2565</v>
       </c>
       <c r="B4" t="s">
-        <v>2413</v>
+        <v>2580</v>
       </c>
       <c r="C4" t="s">
-        <v>2419</v>
+        <v>2597</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2409</v>
+        <v>2565</v>
       </c>
       <c r="B5" t="s">
-        <v>2414</v>
+        <v>2581</v>
       </c>
       <c r="C5" t="s">
-        <v>2420</v>
+        <v>2598</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2409</v>
+        <v>2565</v>
       </c>
       <c r="B6" t="s">
-        <v>2415</v>
+        <v>2582</v>
       </c>
       <c r="C6" t="s">
-        <v>2421</v>
+        <v>2599</v>
       </c>
     </row>
   </sheetData>
@@ -8405,8 +8411,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -8425,7 +8434,7 @@
         <v>2563</v>
       </c>
       <c r="B2" t="s">
-        <v>2567</v>
+        <v>2579</v>
       </c>
       <c r="C2" t="s">
         <v>2584</v>
@@ -8436,7 +8445,7 @@
         <v>2563</v>
       </c>
       <c r="B3" t="s">
-        <v>2568</v>
+        <v>2570</v>
       </c>
       <c r="C3" t="s">
         <v>2585</v>
@@ -8447,7 +8456,7 @@
         <v>2564</v>
       </c>
       <c r="B4" t="s">
-        <v>2569</v>
+        <v>2579</v>
       </c>
       <c r="C4" t="s">
         <v>2586</v>

</xml_diff>